<commit_message>
Changes in Shiny Application
</commit_message>
<xml_diff>
--- a/inst/extdata/example_data_text.xlsx
+++ b/inst/extdata/example_data_text.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveeur-my.sharepoint.com/personal/85304spe_eur_nl/Documents/Documents/mhqol/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_F844377FC3574AFC124848E5AAEAC0011471A05A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC622595-7424-4757-9E57-AD2D2703BE40}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="11_F844377FC3574AFC124848E5AAEAC0011471A05A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52A8B67B-3B1B-4DB2-AD1C-F6A0170DE650}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -286,7 +286,7 @@
     <t>I am very gloomy about my future</t>
   </si>
   <si>
-    <t>I am gloomy about my	future</t>
+    <t>I am gloomy about my future</t>
   </si>
 </sst>
 </file>
@@ -660,11 +660,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="10" max="10" width="76.54296875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B1" t="s">

</xml_diff>